<commit_message>
SPIDR Example fix to product export
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/InternetLoginValues.xlsx
+++ b/src/test/resources/testdata/InternetLoginValues.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Java Framework\testOpsJavaFramework\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testOpsJavaFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA5FDC4-BC58-45C0-8439-A92EE2403539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58E51CD-3C35-4405-BA92-F8900A5EBD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="testCase1" sheetId="1" r:id="rId1"/>
@@ -33,16 +33,16 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Accuride</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
     <t>LoginLabel</t>
   </si>
   <si>
-    <t>ACCURIDE  SUPPLIER</t>
+    <t>groteauto</t>
+  </si>
+  <si>
+    <t>GROTE AUTOMATION</t>
   </si>
 </sst>
 </file>
@@ -390,17 +390,17 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -408,15 +408,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
import and export now working
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/InternetLoginValues.xlsx
+++ b/src/test/resources/testdata/InternetLoginValues.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\testOpsJavaFramework\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58E51CD-3C35-4405-BA92-F8900A5EBD82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424E63EC-FDE3-4030-B1A4-3B681D9AEF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,10 +39,10 @@
     <t>LoginLabel</t>
   </si>
   <si>
-    <t>groteauto</t>
-  </si>
-  <si>
-    <t>GROTE AUTOMATION</t>
+    <t>testSean</t>
+  </si>
+  <si>
+    <t>SEANTEST PROCTOR</t>
   </si>
 </sst>
 </file>
@@ -390,7 +390,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>